<commit_message>
new function to check relation
check_relation is comleted
1. insert code to make_members_info to take a information from relation sheet
2. insert code to check relation to decide_callduty members
3. new function to check relation
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taehunlee/Desktop/duty_schedule_ver2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A13AEF9E-7ED2-F245-BBDF-D586D3A2FFF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6E47F7-468B-664A-8696-E664A44741FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="28720" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3500" windowWidth="28720" windowHeight="17500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hoped_day" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="194">
   <si>
     <t>年度</t>
   </si>
@@ -2506,6 +2506,10 @@
   <si>
     <t>第二</t>
   </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -2667,23 +2671,7 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -9178,10 +9166,10 @@
   </sheetData>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="A3:B32">
-    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
       <formula>WEEKDAY(A3)=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
       <formula>WEEKDAY(A3)=7</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9214,16 +9202,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2915E50-2A83-C34B-9533-BA3C53FB1A92}">
   <dimension ref="A1:W27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F33" sqref="F33"/>
+      <selection pane="bottomRight" activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:23">
+      <c r="A1" t="s">
+        <v>193</v>
+      </c>
       <c r="B1" t="str">
         <f>hoped_day!C2</f>
         <v>北</v>
@@ -9364,7 +9355,7 @@
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -9450,7 +9441,7 @@
         <v>0</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3">
         <v>0</v>
@@ -9500,7 +9491,7 @@
         <v>0</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -9707,7 +9698,7 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -9947,7 +9938,7 @@
         <v>0</v>
       </c>
       <c r="V10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W10">
         <v>0</v>
@@ -10112,7 +10103,7 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -10248,7 +10239,7 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -10384,7 +10375,7 @@
         <v>寺西</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -10583,7 +10574,7 @@
         <v>0</v>
       </c>
       <c r="U19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V19">
         <v>0</v>
@@ -10719,7 +10710,7 @@
         <v>0</v>
       </c>
       <c r="S21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T21">
         <v>0</v>
@@ -10742,7 +10733,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -10763,7 +10754,7 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -20648,10 +20639,10 @@
   </sheetData>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="A2:A32">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>WEEKDAY(A2)=7</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
       <formula>WEEKDAY(A2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20679,11 +20670,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:W1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomRight" activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -20696,9 +20687,9 @@
       <c r="A1" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="12" t="b">
-        <f>relation!B1=hoped_day!C2</f>
-        <v>1</v>
+      <c r="B1" s="12" t="str">
+        <f>hoped_day!C2</f>
+        <v>北</v>
       </c>
       <c r="C1" s="12" t="str">
         <f>hoped_day!D2</f>
@@ -21583,7 +21574,7 @@
         <v>4</v>
       </c>
       <c r="F13" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="15">
         <v>0</v>

</xml_diff>